<commit_message>
Update organizer photos in spreadsheet data
</commit_message>
<xml_diff>
--- a/data/organizers.xlsx
+++ b/data/organizers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-18.04\home\willie\Projects\hackutd-site\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2941BA23-9973-45B3-B8E4-7A38A2D87ADD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE93AF20-8794-4029-B46F-9E7290D49BFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2415" yWindow="2985" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="186">
   <si>
     <t>Willie Chalmers III</t>
   </si>
@@ -521,6 +521,75 @@
   </si>
   <si>
     <t>A valuable member of the HackUTD team.</t>
+  </si>
+  <si>
+    <t>camden_squire.jpg</t>
+  </si>
+  <si>
+    <t>guangze_zu.jpg</t>
+  </si>
+  <si>
+    <t>david_richey.jpg</t>
+  </si>
+  <si>
+    <t>gautam_sapre.jpg</t>
+  </si>
+  <si>
+    <t>pallavi_vayalali.jpg</t>
+  </si>
+  <si>
+    <t>caitlin_tibbetts.jpg</t>
+  </si>
+  <si>
+    <t>sivam_patel.jpg</t>
+  </si>
+  <si>
+    <t>soham_mukerjee.jpg</t>
+  </si>
+  <si>
+    <t>chaithu_dikkala.jpg</t>
+  </si>
+  <si>
+    <t>neha_rode.jpg</t>
+  </si>
+  <si>
+    <t>aditya_guin.jpg</t>
+  </si>
+  <si>
+    <t>austin_luong.jpg</t>
+  </si>
+  <si>
+    <t>rolando_gonzalez.jpg</t>
+  </si>
+  <si>
+    <t>atharv_jain.jpg</t>
+  </si>
+  <si>
+    <t>willie_chalmers iii.jpg</t>
+  </si>
+  <si>
+    <t>sanjana_sivakumar.jpg</t>
+  </si>
+  <si>
+    <t>vishvak_bandi.jpg</t>
+  </si>
+  <si>
+    <t>alexander_osypov.jpg</t>
+  </si>
+  <si>
+    <t>michael_xu.jpg</t>
+  </si>
+  <si>
+    <t>daniel_wang.jpg</t>
+  </si>
+  <si>
+    <t>ishpreet_bhasin.jpg</t>
+  </si>
+  <si>
+    <t>elvina_almeida.jpg</t>
+  </si>
+  <si>
+    <t>abhitej_arora.jpg</t>
   </si>
 </sst>
 </file>
@@ -837,7 +906,7 @@
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25:I25"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -915,7 +984,9 @@
         <v>161</v>
       </c>
       <c r="H2" s="1"/>
-      <c r="I2" s="10"/>
+      <c r="I2" s="10" t="s">
+        <v>163</v>
+      </c>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
@@ -944,7 +1015,9 @@
         <v>162</v>
       </c>
       <c r="H3" s="1"/>
-      <c r="I3" s="10"/>
+      <c r="I3" s="10" t="s">
+        <v>164</v>
+      </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
@@ -973,7 +1046,9 @@
         <v>162</v>
       </c>
       <c r="H4" s="1"/>
-      <c r="I4" s="10"/>
+      <c r="I4" s="10" t="s">
+        <v>165</v>
+      </c>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
@@ -1002,7 +1077,9 @@
         <v>162</v>
       </c>
       <c r="H5" s="1"/>
-      <c r="I5" s="10"/>
+      <c r="I5" s="10" t="s">
+        <v>166</v>
+      </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
@@ -1031,7 +1108,9 @@
         <v>162</v>
       </c>
       <c r="H6" s="1"/>
-      <c r="I6" s="10"/>
+      <c r="I6" s="10" t="s">
+        <v>167</v>
+      </c>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
@@ -1060,7 +1139,9 @@
         <v>159</v>
       </c>
       <c r="H7" s="1"/>
-      <c r="I7" s="10"/>
+      <c r="I7" s="10" t="s">
+        <v>168</v>
+      </c>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
@@ -1089,7 +1170,9 @@
         <v>162</v>
       </c>
       <c r="H8" s="1"/>
-      <c r="I8" s="10"/>
+      <c r="I8" s="10" t="s">
+        <v>169</v>
+      </c>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
@@ -1118,7 +1201,9 @@
         <v>152</v>
       </c>
       <c r="H9" s="1"/>
-      <c r="I9" s="10"/>
+      <c r="I9" s="10" t="s">
+        <v>170</v>
+      </c>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
@@ -1147,7 +1232,9 @@
         <v>162</v>
       </c>
       <c r="H10" s="1"/>
-      <c r="I10" s="10"/>
+      <c r="I10" s="10" t="s">
+        <v>171</v>
+      </c>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
@@ -1176,7 +1263,9 @@
         <v>153</v>
       </c>
       <c r="H11" s="1"/>
-      <c r="I11" s="10"/>
+      <c r="I11" s="10" t="s">
+        <v>172</v>
+      </c>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="12" t="s">
@@ -1207,7 +1296,9 @@
         <v>162</v>
       </c>
       <c r="H12" s="1"/>
-      <c r="I12" s="10"/>
+      <c r="I12" s="10" t="s">
+        <v>173</v>
+      </c>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
@@ -1236,7 +1327,9 @@
         <v>162</v>
       </c>
       <c r="H13" s="1"/>
-      <c r="I13" s="10"/>
+      <c r="I13" s="10" t="s">
+        <v>174</v>
+      </c>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
@@ -1265,7 +1358,9 @@
         <v>160</v>
       </c>
       <c r="H14" s="1"/>
-      <c r="I14" s="10"/>
+      <c r="I14" s="10" t="s">
+        <v>175</v>
+      </c>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
@@ -1293,7 +1388,9 @@
       <c r="G15" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="I15" s="10"/>
+      <c r="I15" s="10" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="16" spans="1:13" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -1320,7 +1417,9 @@
       <c r="H16" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I16" s="12"/>
+      <c r="I16" s="10" t="s">
+        <v>177</v>
+      </c>
       <c r="J16" s="3" t="s">
         <v>4</v>
       </c>
@@ -1334,7 +1433,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>97</v>
       </c>
@@ -1356,8 +1455,11 @@
       <c r="G17" s="5" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I17" s="10" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>99</v>
       </c>
@@ -1379,8 +1481,11 @@
       <c r="G18" s="5" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I18" s="10" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>101</v>
       </c>
@@ -1402,8 +1507,11 @@
       <c r="G19" s="5" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I19" s="10" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>103</v>
       </c>
@@ -1425,8 +1533,11 @@
       <c r="G20" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I20" s="10" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>105</v>
       </c>
@@ -1448,8 +1559,11 @@
       <c r="G21" s="11" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I21" s="10" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>107</v>
       </c>
@@ -1471,8 +1585,11 @@
       <c r="G22" s="11" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I22" s="10" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>109</v>
       </c>
@@ -1494,8 +1611,11 @@
       <c r="G23" s="11" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I23" s="10" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>111</v>
       </c>
@@ -1517,15 +1637,18 @@
       <c r="G24" s="11" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I24" s="10" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="9"/>
       <c r="F25" s="10"/>
       <c r="G25" s="5"/>
     </row>
-    <row r="26" spans="1:7" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C26" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Use default image for officer profiles
</commit_message>
<xml_diff>
--- a/data/organizers.xlsx
+++ b/data/organizers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-18.04\home\willie\Projects\hackutd-site\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE93AF20-8794-4029-B46F-9E7290D49BFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CEC5C91-DCF6-4401-BD04-8671CFF3FD9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2415" yWindow="2985" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-1365" yWindow="3090" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Organizers" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="181">
   <si>
     <t>Willie Chalmers III</t>
   </si>
@@ -526,9 +526,6 @@
     <t>camden_squire.jpg</t>
   </si>
   <si>
-    <t>guangze_zu.jpg</t>
-  </si>
-  <si>
     <t>david_richey.jpg</t>
   </si>
   <si>
@@ -559,15 +556,9 @@
     <t>austin_luong.jpg</t>
   </si>
   <si>
-    <t>rolando_gonzalez.jpg</t>
-  </si>
-  <si>
     <t>atharv_jain.jpg</t>
   </si>
   <si>
-    <t>willie_chalmers iii.jpg</t>
-  </si>
-  <si>
     <t>sanjana_sivakumar.jpg</t>
   </si>
   <si>
@@ -577,19 +568,13 @@
     <t>alexander_osypov.jpg</t>
   </si>
   <si>
-    <t>michael_xu.jpg</t>
-  </si>
-  <si>
     <t>daniel_wang.jpg</t>
   </si>
   <si>
-    <t>ishpreet_bhasin.jpg</t>
-  </si>
-  <si>
-    <t>elvina_almeida.jpg</t>
-  </si>
-  <si>
-    <t>abhitej_arora.jpg</t>
+    <t>officer_default.svg</t>
+  </si>
+  <si>
+    <t>willie_chalmers.jpg</t>
   </si>
 </sst>
 </file>
@@ -905,8 +890,8 @@
   </sheetPr>
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1016,7 +1001,7 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="10" t="s">
-        <v>164</v>
+        <v>179</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
@@ -1047,7 +1032,7 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
@@ -1078,7 +1063,7 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
@@ -1109,7 +1094,7 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
@@ -1140,7 +1125,7 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
@@ -1171,7 +1156,7 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
@@ -1202,7 +1187,7 @@
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
@@ -1233,7 +1218,7 @@
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
@@ -1264,7 +1249,7 @@
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
@@ -1297,7 +1282,7 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
@@ -1328,7 +1313,7 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
@@ -1359,7 +1344,7 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="10" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
@@ -1389,7 +1374,7 @@
         <v>162</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -1418,7 +1403,7 @@
         <v>3</v>
       </c>
       <c r="I16" s="10" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="J16" s="3" t="s">
         <v>4</v>
@@ -1456,7 +1441,7 @@
         <v>156</v>
       </c>
       <c r="I17" s="10" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -1482,7 +1467,7 @@
         <v>157</v>
       </c>
       <c r="I18" s="10" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -1508,7 +1493,7 @@
         <v>158</v>
       </c>
       <c r="I19" s="10" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -1534,7 +1519,7 @@
         <v>155</v>
       </c>
       <c r="I20" s="10" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -1560,7 +1545,7 @@
         <v>162</v>
       </c>
       <c r="I21" s="10" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -1586,7 +1571,7 @@
         <v>162</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -1612,7 +1597,7 @@
         <v>162</v>
       </c>
       <c r="I23" s="10" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -1638,7 +1623,7 @@
         <v>162</v>
       </c>
       <c r="I24" s="10" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Fix excel typo and sort organizers
</commit_message>
<xml_diff>
--- a/data/organizers.xlsx
+++ b/data/organizers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-18.04\home\willie\Projects\hackutd-site\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WebProjects\hackutd.github.io\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CEC5C91-DCF6-4401-BD04-8671CFF3FD9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C54EB909-CDDD-4CC3-A727-77314B2A4B3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1365" yWindow="3090" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Organizers" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="180">
   <si>
     <t>Willie Chalmers III</t>
   </si>
@@ -398,9 +398,6 @@
   </si>
   <si>
     <t>HackUTD Logistics Coordinator</t>
-  </si>
-  <si>
-    <t>HackUTD Logistics Coorindator</t>
   </si>
   <si>
     <t>HackUTD Technical Coordinator</t>
@@ -890,8 +887,8 @@
   </sheetPr>
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -899,7 +896,7 @@
     <col min="1" max="1" width="9.5703125" customWidth="1"/>
     <col min="2" max="2" width="11.140625" customWidth="1"/>
     <col min="3" max="3" width="17.85546875" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="4" max="4" width="81.28515625" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" customWidth="1"/>
     <col min="6" max="6" width="9.140625" customWidth="1"/>
     <col min="7" max="7" width="36" style="6" customWidth="1"/>
@@ -954,23 +951,23 @@
         <v>69</v>
       </c>
       <c r="C2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
@@ -985,23 +982,23 @@
         <v>71</v>
       </c>
       <c r="C3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>113</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
@@ -1016,23 +1013,23 @@
         <v>73</v>
       </c>
       <c r="C4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>114</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
@@ -1047,7 +1044,7 @@
         <v>75</v>
       </c>
       <c r="C5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>115</v>
@@ -1056,14 +1053,14 @@
         <v>1</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
@@ -1078,23 +1075,23 @@
         <v>77</v>
       </c>
       <c r="C6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>116</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
@@ -1109,23 +1106,23 @@
         <v>79</v>
       </c>
       <c r="C7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>117</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
@@ -1140,7 +1137,7 @@
         <v>81</v>
       </c>
       <c r="C8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>118</v>
@@ -1149,14 +1146,14 @@
         <v>1</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
@@ -1171,7 +1168,7 @@
         <v>83</v>
       </c>
       <c r="C9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>119</v>
@@ -1180,14 +1177,14 @@
         <v>1</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
@@ -1202,7 +1199,7 @@
         <v>85</v>
       </c>
       <c r="C10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>119</v>
@@ -1211,14 +1208,14 @@
         <v>1</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
@@ -1233,7 +1230,7 @@
         <v>87</v>
       </c>
       <c r="C11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>119</v>
@@ -1242,19 +1239,19 @@
         <v>1</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="M11" s="3"/>
     </row>
@@ -1266,7 +1263,7 @@
         <v>89</v>
       </c>
       <c r="C12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>120</v>
@@ -1275,14 +1272,14 @@
         <v>1</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
@@ -1297,7 +1294,7 @@
         <v>91</v>
       </c>
       <c r="C13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>121</v>
@@ -1306,14 +1303,14 @@
         <v>1</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
@@ -1328,7 +1325,7 @@
         <v>93</v>
       </c>
       <c r="C14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>118</v>
@@ -1337,14 +1334,14 @@
         <v>1</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
@@ -1359,22 +1356,22 @@
         <v>95</v>
       </c>
       <c r="C15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -1382,28 +1379,28 @@
         <v>96</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C16" t="s">
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>3</v>
       </c>
       <c r="I16" s="10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J16" s="3" t="s">
         <v>4</v>
@@ -1426,7 +1423,7 @@
         <v>98</v>
       </c>
       <c r="C17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D17" t="s">
         <v>121</v>
@@ -1435,13 +1432,13 @@
         <v>1</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I17" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -1452,7 +1449,7 @@
         <v>100</v>
       </c>
       <c r="C18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D18" t="s">
         <v>120</v>
@@ -1461,13 +1458,13 @@
         <v>1</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I18" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -1478,7 +1475,7 @@
         <v>102</v>
       </c>
       <c r="C19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D19" t="s">
         <v>118</v>
@@ -1487,13 +1484,13 @@
         <v>1</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I19" s="10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -1504,22 +1501,22 @@
         <v>104</v>
       </c>
       <c r="C20" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I20" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -1530,22 +1527,22 @@
         <v>106</v>
       </c>
       <c r="C21" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D21" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I21" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -1556,7 +1553,7 @@
         <v>108</v>
       </c>
       <c r="C22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D22" t="s">
         <v>118</v>
@@ -1565,13 +1562,13 @@
         <v>2</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -1582,7 +1579,7 @@
         <v>110</v>
       </c>
       <c r="C23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D23" t="s">
         <v>119</v>
@@ -1591,13 +1588,13 @@
         <v>2</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I23" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -1608,7 +1605,7 @@
         <v>112</v>
       </c>
       <c r="C24" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D24" t="s">
         <v>120</v>
@@ -1617,13 +1614,13 @@
         <v>2</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I24" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Fix position names and remove position info from cards
</commit_message>
<xml_diff>
--- a/data/organizers.xlsx
+++ b/data/organizers.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WebProjects\hackutd.github.io\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C54EB909-CDDD-4CC3-A727-77314B2A4B3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E7BD31-BC4A-4509-9ADE-D3CED4BA69CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -388,21 +388,6 @@
     <t>HackUTD Marketing Leader</t>
   </si>
   <si>
-    <t>HackUTD Experience Coordinator</t>
-  </si>
-  <si>
-    <t>HackUTD Marketing Coordinator</t>
-  </si>
-  <si>
-    <t>HackUTD Industry Coordinator</t>
-  </si>
-  <si>
-    <t>HackUTD Logistics Coordinator</t>
-  </si>
-  <si>
-    <t>HackUTD Technical Coordinator</t>
-  </si>
-  <si>
     <t>Director of HackUTD</t>
   </si>
   <si>
@@ -502,9 +487,6 @@
     <t xml:space="preserve">Sanjana is a sophomore majoring in computer science. She is logistics coordinator for hackUTD. In her free time she loves to dance, make tik toks, and spend time with friends and family! </t>
   </si>
   <si>
-    <t>Vishvak is a HackUTD Industry Coordinator and is studying Computer Science at UT Dallas. In his free time he enjoys playing video games and listening to music. He also enjoys trying out new technology and crashing his drones.</t>
-  </si>
-  <si>
     <t>Alex is a Data Science student. Alex likes to play video games, critique shows and movies, and practice martial arts.</t>
   </si>
   <si>
@@ -572,6 +554,24 @@
   </si>
   <si>
     <t>willie_chalmers.jpg</t>
+  </si>
+  <si>
+    <t>HackUTD Experience Coordinators</t>
+  </si>
+  <si>
+    <t>HackUTD Marketing Coordinators</t>
+  </si>
+  <si>
+    <t>HackUTD Industry Coordinators</t>
+  </si>
+  <si>
+    <t>Vishvak is a HackUTD Industry Coordinators and is studying Computer Science at UT Dallas. In his free time he enjoys playing video games and listening to music. He also enjoys trying out new technology and crashing his drones.</t>
+  </si>
+  <si>
+    <t>HackUTD Logistics Coordinators</t>
+  </si>
+  <si>
+    <t>HackUTD Technical Coordinators</t>
   </si>
 </sst>
 </file>
@@ -888,7 +888,7 @@
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -951,23 +951,23 @@
         <v>69</v>
       </c>
       <c r="C2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="10" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
@@ -982,23 +982,23 @@
         <v>71</v>
       </c>
       <c r="C3" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>113</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="10" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
@@ -1013,23 +1013,23 @@
         <v>73</v>
       </c>
       <c r="C4" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>114</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="10" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
@@ -1044,7 +1044,7 @@
         <v>75</v>
       </c>
       <c r="C5" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>115</v>
@@ -1053,14 +1053,14 @@
         <v>1</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="10" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
@@ -1075,23 +1075,23 @@
         <v>77</v>
       </c>
       <c r="C6" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>116</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="10" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
@@ -1106,23 +1106,23 @@
         <v>79</v>
       </c>
       <c r="C7" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>117</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="10" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
@@ -1137,23 +1137,23 @@
         <v>81</v>
       </c>
       <c r="C8" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>118</v>
+        <v>174</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>1</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="10" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
@@ -1168,23 +1168,23 @@
         <v>83</v>
       </c>
       <c r="C9" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>119</v>
+        <v>175</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="10" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
@@ -1199,23 +1199,23 @@
         <v>85</v>
       </c>
       <c r="C10" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>119</v>
+        <v>175</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="10" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
@@ -1230,28 +1230,28 @@
         <v>87</v>
       </c>
       <c r="C11" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>119</v>
+        <v>175</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="10" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="12" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="M11" s="3"/>
     </row>
@@ -1263,23 +1263,23 @@
         <v>89</v>
       </c>
       <c r="C12" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>120</v>
+        <v>176</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="10" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
@@ -1294,23 +1294,23 @@
         <v>91</v>
       </c>
       <c r="C13" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>121</v>
+        <v>178</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="10" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
@@ -1325,23 +1325,23 @@
         <v>93</v>
       </c>
       <c r="C14" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>118</v>
+        <v>174</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="10" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
@@ -1356,22 +1356,22 @@
         <v>95</v>
       </c>
       <c r="C15" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>121</v>
+        <v>178</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -1379,28 +1379,28 @@
         <v>96</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C16" t="s">
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>122</v>
+        <v>179</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>3</v>
       </c>
       <c r="I16" s="10" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="J16" s="3" t="s">
         <v>4</v>
@@ -1423,22 +1423,22 @@
         <v>98</v>
       </c>
       <c r="C17" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D17" t="s">
-        <v>121</v>
+        <v>178</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="I17" s="10" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -1449,22 +1449,22 @@
         <v>100</v>
       </c>
       <c r="C18" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D18" t="s">
-        <v>120</v>
+        <v>176</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>156</v>
+        <v>177</v>
       </c>
       <c r="I18" s="10" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -1475,22 +1475,22 @@
         <v>102</v>
       </c>
       <c r="C19" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D19" t="s">
-        <v>118</v>
+        <v>174</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="I19" s="10" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -1501,22 +1501,22 @@
         <v>104</v>
       </c>
       <c r="C20" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D20" t="s">
-        <v>122</v>
+        <v>179</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F20" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="G20" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="G20" s="5" t="s">
-        <v>154</v>
-      </c>
       <c r="I20" s="10" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -1527,22 +1527,22 @@
         <v>106</v>
       </c>
       <c r="C21" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D21" t="s">
-        <v>122</v>
+        <v>179</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="I21" s="10" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -1553,22 +1553,22 @@
         <v>108</v>
       </c>
       <c r="C22" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D22" t="s">
-        <v>118</v>
+        <v>174</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>2</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -1579,22 +1579,22 @@
         <v>110</v>
       </c>
       <c r="C23" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D23" t="s">
-        <v>119</v>
+        <v>175</v>
       </c>
       <c r="E23" s="9" t="s">
         <v>2</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="I23" s="10" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -1605,22 +1605,22 @@
         <v>112</v>
       </c>
       <c r="C24" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="D24" t="s">
-        <v>120</v>
+        <v>176</v>
       </c>
       <c r="E24" s="9" t="s">
         <v>2</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="I24" s="10" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
updated team and archived sites
</commit_message>
<xml_diff>
--- a/data/organizers.xlsx
+++ b/data/organizers.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abdul\Desktop\hackutd\hackutd-site\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/namtruong/Projects/hackutd-site/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B1E1E61-9DF1-489F-A9D3-3D7BC833E317}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A32ECB1F-CB04-C844-8625-59DDC297136D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29190" yWindow="-12015" windowWidth="17280" windowHeight="9030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Organizers" sheetId="1" r:id="rId1"/>
+    <sheet name="Organizers" sheetId="5" r:id="rId1"/>
     <sheet name="Events" sheetId="2" r:id="rId2"/>
     <sheet name="Workshops" sheetId="3" r:id="rId3"/>
+    <sheet name="Organizers vii" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="180">
   <si>
     <t>2020s</t>
   </si>
@@ -439,9 +440,6 @@
     <t>Abdullah Hasani</t>
   </si>
   <si>
-    <t>Nam Troung</t>
-  </si>
-  <si>
     <t>HackUTD Technical Coordinator</t>
   </si>
   <si>
@@ -476,6 +474,105 @@
   </si>
   <si>
     <t>soham_mukerjee.jpg</t>
+  </si>
+  <si>
+    <t>Nam Truong</t>
+  </si>
+  <si>
+    <t>Rolando </t>
+  </si>
+  <si>
+    <t>Ishpreet </t>
+  </si>
+  <si>
+    <t>Ishpreet Bhasin</t>
+  </si>
+  <si>
+    <t>Thais</t>
+  </si>
+  <si>
+    <t>Campanac-Climent</t>
+  </si>
+  <si>
+    <t>Jariel</t>
+  </si>
+  <si>
+    <t>Gojar</t>
+  </si>
+  <si>
+    <t>Arora</t>
+  </si>
+  <si>
+    <t>Aadit</t>
+  </si>
+  <si>
+    <t>Meenege</t>
+  </si>
+  <si>
+    <t>Alina</t>
+  </si>
+  <si>
+    <t>Tieu</t>
+  </si>
+  <si>
+    <t>Shreya</t>
+  </si>
+  <si>
+    <t>Parihar</t>
+  </si>
+  <si>
+    <t>Dylan</t>
+  </si>
+  <si>
+    <t>Nguyen</t>
+  </si>
+  <si>
+    <t>Neal</t>
+  </si>
+  <si>
+    <t>Gandhi</t>
+  </si>
+  <si>
+    <t>Sameer</t>
+  </si>
+  <si>
+    <t>Haq</t>
+  </si>
+  <si>
+    <t>Arjun</t>
+  </si>
+  <si>
+    <t>Venkat</t>
+  </si>
+  <si>
+    <t>Thais Campanac-Climent</t>
+  </si>
+  <si>
+    <t>Jariel Gojar</t>
+  </si>
+  <si>
+    <t>Shreya Parihar</t>
+  </si>
+  <si>
+    <t>Dylan Nguyen</t>
+  </si>
+  <si>
+    <t>Arjun Venkat</t>
+  </si>
+  <si>
+    <t>Sameer Haq</t>
+  </si>
+  <si>
+    <t>Neal Gandhi</t>
+  </si>
+  <si>
+    <t>Alina Tieu</t>
+  </si>
+  <si>
+    <t>Aadit Meenege</t>
+  </si>
+  <si>
+    <t>2021s</t>
   </si>
 </sst>
 </file>
@@ -808,28 +905,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D93BD866-5CC6-084B-B5E9-3B946F40E9F8}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="32" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" customWidth="1"/>
-    <col min="3" max="3" width="17.88671875" customWidth="1"/>
-    <col min="4" max="4" width="39.44140625" customWidth="1"/>
+    <col min="1" max="1" width="9.5" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" customWidth="1"/>
+    <col min="4" max="4" width="39.5" customWidth="1"/>
     <col min="5" max="5" width="10.6640625" customWidth="1"/>
-    <col min="6" max="6" width="9.109375" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" customWidth="1"/>
     <col min="7" max="7" width="36" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>60</v>
       </c>
@@ -870,21 +967,21 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="D2" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="D2" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="E2" s="16" t="s">
-        <v>0</v>
+      <c r="E2" s="17" t="s">
+        <v>179</v>
       </c>
       <c r="F2" s="13" t="s">
         <v>122</v>
@@ -892,26 +989,26 @@
       <c r="G2" s="15"/>
       <c r="H2" s="14"/>
       <c r="I2" s="13" t="s">
-        <v>147</v>
+        <v>123</v>
       </c>
       <c r="J2" s="14"/>
       <c r="M2" s="3"/>
     </row>
-    <row r="3" spans="1:13" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="14" t="s">
-        <v>92</v>
+        <v>162</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>93</v>
+        <v>163</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="D3" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="D3" s="14" t="s">
         <v>100</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>1</v>
+        <v>179</v>
       </c>
       <c r="F3" s="13" t="s">
         <v>122</v>
@@ -924,20 +1021,20 @@
       <c r="J3" s="14"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:13" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>109</v>
+        <v>72</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>108</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="17" t="s">
         <v>0</v>
       </c>
       <c r="F4" s="13" t="s">
@@ -946,25 +1043,25 @@
       <c r="G4" s="11"/>
       <c r="H4" s="18"/>
       <c r="I4" s="13" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="J4" s="14"/>
     </row>
-    <row r="5" spans="1:13" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>113</v>
+    <row r="5" spans="1:13" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>168</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>174</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="E5" s="16" t="s">
-        <v>0</v>
+      <c r="E5" s="17" t="s">
+        <v>179</v>
       </c>
       <c r="F5" s="13" t="s">
         <v>122</v>
@@ -972,26 +1069,26 @@
       <c r="G5" s="11"/>
       <c r="H5" s="18"/>
       <c r="I5" s="13" t="s">
-        <v>144</v>
+        <v>123</v>
       </c>
       <c r="J5" s="14"/>
       <c r="M5" s="3"/>
     </row>
-    <row r="6" spans="1:13" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>101</v>
+    <row r="6" spans="1:13" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>102</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>1</v>
+        <v>179</v>
       </c>
       <c r="F6" s="13" t="s">
         <v>122</v>
@@ -1004,21 +1101,21 @@
       <c r="J6" s="14"/>
       <c r="M6" s="3"/>
     </row>
-    <row r="7" spans="1:13" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="E7" s="16" t="s">
-        <v>0</v>
+    <row r="7" spans="1:13" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>164</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>179</v>
       </c>
       <c r="F7" s="13" t="s">
         <v>122</v>
@@ -1026,27 +1123,27 @@
       <c r="G7" s="15"/>
       <c r="H7" s="18"/>
       <c r="I7" s="13" t="s">
-        <v>145</v>
+        <v>123</v>
       </c>
       <c r="J7" s="14"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
     </row>
-    <row r="8" spans="1:13" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>111</v>
+    <row r="8" spans="1:13" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>109</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="E8" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="E8" s="17" t="s">
         <v>0</v>
       </c>
       <c r="F8" s="13" t="s">
@@ -1055,26 +1152,26 @@
       <c r="G8" s="15"/>
       <c r="H8" s="18"/>
       <c r="I8" s="13" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="J8" s="14"/>
       <c r="M8" s="3"/>
     </row>
-    <row r="9" spans="1:13" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>135</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>136</v>
+    <row r="9" spans="1:13" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>158</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>101</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>1</v>
+        <v>179</v>
       </c>
       <c r="F9" s="13" t="s">
         <v>122</v>
@@ -1089,21 +1186,21 @@
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
     </row>
-    <row r="10" spans="1:13" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="14" t="s">
-        <v>126</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>133</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>136</v>
+    <row r="10" spans="1:13" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>101</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>1</v>
+        <v>179</v>
       </c>
       <c r="F10" s="13" t="s">
         <v>122</v>
@@ -1118,21 +1215,21 @@
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
     </row>
-    <row r="11" spans="1:13" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>136</v>
+    <row r="11" spans="1:13" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>101</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11" s="13" t="s">
         <v>122</v>
@@ -1140,25 +1237,25 @@
       <c r="G11" s="15"/>
       <c r="H11" s="18"/>
       <c r="I11" s="13" t="s">
-        <v>123</v>
+        <v>144</v>
       </c>
       <c r="J11" s="14"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
     </row>
-    <row r="12" spans="1:13" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>117</v>
+    <row r="12" spans="1:13" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>119</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E12" s="17" t="s">
         <v>1</v>
@@ -1176,21 +1273,21 @@
       <c r="L12" s="12"/>
       <c r="M12" s="3"/>
     </row>
-    <row r="13" spans="1:13" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="14" t="s">
-        <v>86</v>
+        <v>130</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>0</v>
+        <v>131</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>1</v>
       </c>
       <c r="F13" s="13" t="s">
         <v>122</v>
@@ -1198,28 +1295,28 @@
       <c r="G13" s="11"/>
       <c r="H13" s="14"/>
       <c r="I13" s="13" t="s">
-        <v>146</v>
+        <v>123</v>
       </c>
       <c r="J13" s="14"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
     </row>
-    <row r="14" spans="1:13" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>112</v>
+    <row r="14" spans="1:13" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>134</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>0</v>
+        <v>135</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>1</v>
       </c>
       <c r="F14" s="13" t="s">
         <v>122</v>
@@ -1234,21 +1331,21 @@
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
     </row>
-    <row r="15" spans="1:13" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>107</v>
+    <row r="15" spans="1:13" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>171</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>99</v>
+        <v>135</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>0</v>
+        <v>179</v>
       </c>
       <c r="F15" s="13" t="s">
         <v>122</v>
@@ -1256,28 +1353,28 @@
       <c r="G15" s="11"/>
       <c r="H15" s="18"/>
       <c r="I15" s="13" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="J15" s="14"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
     </row>
-    <row r="16" spans="1:13" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>125</v>
+    <row r="16" spans="1:13" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>135</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>121</v>
+        <v>179</v>
       </c>
       <c r="F16" s="13" t="s">
         <v>122</v>
@@ -1285,28 +1382,28 @@
       <c r="G16" s="15"/>
       <c r="H16" s="18"/>
       <c r="I16" s="13" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
       <c r="J16" s="14"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
     </row>
-    <row r="17" spans="1:13" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="14" t="s">
-        <v>68</v>
+        <v>148</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>106</v>
+        <v>81</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>112</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>121</v>
+        <v>0</v>
       </c>
       <c r="F17" s="13" t="s">
         <v>122</v>
@@ -1314,28 +1411,28 @@
       <c r="G17" s="11"/>
       <c r="H17" s="18"/>
       <c r="I17" s="13" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="J17" s="14"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
     </row>
-    <row r="18" spans="1:13" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="B18" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>97</v>
+        <v>149</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>99</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18" s="13" t="s">
         <v>122</v>
@@ -1343,25 +1440,25 @@
       <c r="G18" s="11"/>
       <c r="H18" s="18"/>
       <c r="I18" s="13" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="J18" s="14"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
     </row>
-    <row r="19" spans="1:13" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="14" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>96</v>
+        <v>124</v>
       </c>
       <c r="E19" s="17" t="s">
         <v>121</v>
@@ -1372,103 +1469,62 @@
       <c r="G19" s="11"/>
       <c r="H19" s="18"/>
       <c r="I19" s="13" t="s">
-        <v>123</v>
+        <v>139</v>
       </c>
       <c r="J19" s="14"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
     </row>
-    <row r="20" spans="1:13" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="B20" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="D20" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="E20" s="17" t="s">
-        <v>120</v>
-      </c>
-      <c r="F20" s="13" t="s">
-        <v>122</v>
-      </c>
+    <row r="20" spans="1:13" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F20" s="13"/>
       <c r="G20" s="11"/>
       <c r="H20" s="18"/>
-      <c r="I20" s="13" t="s">
-        <v>123</v>
-      </c>
+      <c r="I20" s="13"/>
       <c r="J20" s="14"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
     </row>
-    <row r="21" spans="1:13" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="B21" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="D21" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="E21" s="17" t="s">
-        <v>120</v>
-      </c>
-      <c r="F21" s="13" t="s">
-        <v>122</v>
-      </c>
+    <row r="21" spans="1:13" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="G21" s="15"/>
       <c r="H21" s="18"/>
-      <c r="I21" s="13" t="s">
-        <v>137</v>
-      </c>
+      <c r="I21" s="13"/>
       <c r="J21" s="14"/>
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
     </row>
-    <row r="22" spans="1:13" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E22" s="5"/>
+    <row r="22" spans="1:13" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D22" s="2"/>
+      <c r="E22" s="9"/>
       <c r="F22" s="10"/>
       <c r="G22" s="11"/>
       <c r="I22" s="10"/>
     </row>
-    <row r="23" spans="1:13" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E23" s="9"/>
       <c r="F23" s="10"/>
       <c r="G23" s="11"/>
       <c r="I23" s="10"/>
     </row>
-    <row r="24" spans="1:13" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E24" s="9"/>
       <c r="F24" s="10"/>
       <c r="G24" s="11"/>
       <c r="I24" s="10"/>
     </row>
-    <row r="25" spans="1:13" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="9"/>
       <c r="F25" s="10"/>
       <c r="G25" s="5"/>
     </row>
-    <row r="26" spans="1:13" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C26" s="5"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M21">
-    <sortCondition descending="1" ref="M2:M21"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1482,16 +1538,16 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="18.33203125" customWidth="1"/>
-    <col min="2" max="2" width="62.5546875" customWidth="1"/>
-    <col min="3" max="3" width="12.5546875" customWidth="1"/>
+    <col min="2" max="2" width="62.5" customWidth="1"/>
+    <col min="3" max="3" width="12.5" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
     <col min="5" max="5" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
@@ -1514,7 +1570,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1537,7 +1593,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
         <v>50</v>
       </c>
@@ -1552,7 +1608,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -1575,7 +1631,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1598,7 +1654,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1621,7 +1677,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -1644,7 +1700,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="5" t="s">
         <v>48</v>
       </c>
@@ -1661,7 +1717,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1684,7 +1740,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -1707,7 +1763,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1730,7 +1786,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="5" t="s">
         <v>46</v>
       </c>
@@ -1767,17 +1823,17 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="32" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="27.5546875" customWidth="1"/>
-    <col min="2" max="2" width="36.109375" style="6" customWidth="1"/>
+    <col min="1" max="1" width="27.5" customWidth="1"/>
+    <col min="2" max="2" width="36.1640625" style="6" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" customWidth="1"/>
     <col min="5" max="5" width="15.33203125" customWidth="1"/>
-    <col min="6" max="6" width="19.88671875" customWidth="1"/>
+    <col min="6" max="6" width="19.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -1797,7 +1853,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
         <v>38</v>
       </c>
@@ -1817,7 +1873,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
         <v>54</v>
       </c>
@@ -1837,7 +1893,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
         <v>55</v>
       </c>
@@ -1857,7 +1913,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
         <v>56</v>
       </c>
@@ -1877,7 +1933,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
         <v>57</v>
       </c>
@@ -1897,7 +1953,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="5" t="s">
         <v>58</v>
       </c>
@@ -1917,7 +1973,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="5" t="s">
         <v>59</v>
       </c>
@@ -1940,4 +1996,672 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:M26"/>
+  <sheetViews>
+    <sheetView zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection sqref="A1:M1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="32" customHeight="1" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="9.5" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" customWidth="1"/>
+    <col min="4" max="4" width="39.5" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" customWidth="1"/>
+    <col min="7" max="7" width="36" style="6" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="G2" s="15"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="J2" s="14"/>
+      <c r="M2" s="3"/>
+    </row>
+    <row r="3" spans="1:13" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="G3" s="15"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="J3" s="14"/>
+      <c r="M3" s="3"/>
+    </row>
+    <row r="4" spans="1:13" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="G4" s="11"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="J4" s="14"/>
+    </row>
+    <row r="5" spans="1:13" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="G5" s="11"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="J5" s="14"/>
+      <c r="M5" s="3"/>
+    </row>
+    <row r="6" spans="1:13" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="G6" s="15"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="J6" s="14"/>
+      <c r="M6" s="3"/>
+    </row>
+    <row r="7" spans="1:13" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="G7" s="15"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="J7" s="14"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+    </row>
+    <row r="8" spans="1:13" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="G8" s="15"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="J8" s="14"/>
+      <c r="M8" s="3"/>
+    </row>
+    <row r="9" spans="1:13" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="G9" s="11"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="J9" s="14"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+    </row>
+    <row r="10" spans="1:13" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="G10" s="15"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="J10" s="14"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+    </row>
+    <row r="11" spans="1:13" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="G11" s="15"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="J11" s="14"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+    </row>
+    <row r="12" spans="1:13" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="G12" s="15"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="J12" s="14"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="3"/>
+    </row>
+    <row r="13" spans="1:13" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="G13" s="11"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="J13" s="14"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+    </row>
+    <row r="14" spans="1:13" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="G14" s="11"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="J14" s="14"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+    </row>
+    <row r="15" spans="1:13" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="G15" s="11"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="J15" s="14"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+    </row>
+    <row r="16" spans="1:13" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="G16" s="15"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="J16" s="14"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+    </row>
+    <row r="17" spans="1:13" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="G17" s="11"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="J17" s="14"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+    </row>
+    <row r="18" spans="1:13" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="G18" s="11"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="J18" s="14"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+    </row>
+    <row r="19" spans="1:13" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="G19" s="11"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="J19" s="14"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+    </row>
+    <row r="20" spans="1:13" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="G20" s="11"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="J20" s="14"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+    </row>
+    <row r="21" spans="1:13" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="G21" s="15"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="J21" s="14"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+    </row>
+    <row r="22" spans="1:13" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D22" s="2"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="11"/>
+      <c r="I22" s="10"/>
+    </row>
+    <row r="23" spans="1:13" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E23" s="9"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="11"/>
+      <c r="I23" s="10"/>
+    </row>
+    <row r="24" spans="1:13" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E24" s="9"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="11"/>
+      <c r="I24" s="10"/>
+    </row>
+    <row r="25" spans="1:13" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="5"/>
+    </row>
+    <row r="26" spans="1:13" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C26" s="5"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M21">
+    <sortCondition descending="1" ref="M2:M21"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>